<commit_message>
added english version of Julys resume
</commit_message>
<xml_diff>
--- a/yz.xlsx
+++ b/yz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Library/Containers/com.panic.transmit.mas/Data/Library/Caches/Transmit/01393BA1-448B-4D49-9DA3-0EBBF7DCCCC6/192.168.1.19/datalus/weiyu/git/cv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Library/Containers/com.panic.transmit.mas/Data/Library/Caches/Transmit/CAF793A7-38EE-45CC-8FBF-0CEB23F6C7A8/192.168.1.19/datalus/weiyu/git/cv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B09425-E208-2941-9AE7-479B25C75A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9B5C5E-D548-E849-866C-655461907946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9800" yWindow="9440" windowWidth="26900" windowHeight="15040" xr2:uid="{49BEF855-14FC-304C-9B93-8FA563204E38}"/>
+    <workbookView xWindow="9800" yWindow="9440" windowWidth="26900" windowHeight="15040" activeTab="1" xr2:uid="{49BEF855-14FC-304C-9B93-8FA563204E38}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="3" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="language_skills" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="OLE_LINK52" localSheetId="1">english_version!$C$7</definedName>
+    <definedName name="OLE_LINK52" localSheetId="1">english_version!$C$8</definedName>
     <definedName name="OLE_LINK52" localSheetId="0">main!$C$8</definedName>
-    <definedName name="OLE_LINK65" localSheetId="1">english_version!$D$9</definedName>
+    <definedName name="OLE_LINK65" localSheetId="1">english_version!$D$10</definedName>
     <definedName name="OLE_LINK65" localSheetId="0">main!$D$10</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="78">
   <si>
     <t>loc</t>
   </si>
@@ -369,9 +369,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -409,7 +409,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -515,7 +515,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -657,7 +657,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -667,9 +667,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D4E204-A097-E246-8420-89EA1CD35275}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1372,11 +1372,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BA8E4E2-29FC-6B44-964A-B9A6D1C8B589}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1489,26 +1489,23 @@
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>73</v>
+      <c r="C4" t="s">
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
         <v>71</v>
       </c>
       <c r="F4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="G4">
-        <v>9999</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>72</v>
+        <v>2023</v>
+      </c>
+      <c r="H4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1518,23 +1515,23 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>39</v>
+      <c r="C5" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="F5">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="G5">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1544,29 +1541,23 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
+      <c r="C6" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F6">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="G6">
-        <v>2019</v>
-      </c>
-      <c r="H6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" t="s">
-        <v>10</v>
+        <v>2020</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1577,10 +1568,10 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
         <v>24</v>
@@ -1589,13 +1580,13 @@
         <v>2018</v>
       </c>
       <c r="G7">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="H7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I7" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="J7" t="s">
         <v>10</v>
@@ -1609,22 +1600,22 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
         <v>24</v>
       </c>
       <c r="F8">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="G8">
         <v>2018</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I8" t="s">
         <v>10</v>
@@ -1635,28 +1626,28 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>33</v>
+      <c r="C9" t="s">
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F9">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="G9">
-        <v>9999</v>
+        <v>2018</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="I9" t="s">
         <v>10</v>
@@ -1673,22 +1664,22 @@
         <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F10">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="G10">
-        <v>2017</v>
+        <v>9999</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s">
         <v>10</v>
@@ -1705,25 +1696,25 @@
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
         <v>27</v>
       </c>
       <c r="F11">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="G11">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="H11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="J11" t="s">
         <v>10</v>
@@ -1737,25 +1728,25 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="F12">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="G12">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="H12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I12" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="J12" t="s">
         <v>10</v>
@@ -1763,28 +1754,28 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>49</v>
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="F13">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="G13">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="H13" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="I13" t="s">
         <v>10</v>
@@ -1798,22 +1789,22 @@
         <v>47</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
         <v>23</v>
       </c>
       <c r="F14">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="G14">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="H14" t="s">
         <v>10</v>
@@ -1830,13 +1821,13 @@
         <v>47</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
         <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
         <v>23</v>
@@ -1859,25 +1850,25 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F16">
-        <v>2017</v>
+        <v>2011</v>
       </c>
       <c r="G16">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="H16" t="s">
         <v>10</v>
@@ -1897,19 +1888,19 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F17">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="G17">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="H17" t="s">
         <v>10</v>
@@ -1932,7 +1923,7 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
         <v>23</v>
@@ -1964,7 +1955,7 @@
         <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
         <v>23</v>
@@ -1996,16 +1987,16 @@
         <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
         <v>23</v>
       </c>
       <c r="F20">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="G20">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="H20" t="s">
         <v>10</v>
@@ -2028,7 +2019,7 @@
         <v>49</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
         <v>23</v>
@@ -2046,6 +2037,38 @@
         <v>10</v>
       </c>
       <c r="J21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22">
+        <v>2011</v>
+      </c>
+      <c r="G22">
+        <v>2011</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>